<commit_message>
Finished up functionality. Need style and make protable
</commit_message>
<xml_diff>
--- a/TimeInTimeOut.xlsx
+++ b/TimeInTimeOut.xlsx
@@ -1,39 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith Rich\Documents\PythonScripts\TimeCard\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EE7110-0FFD-443F-A20E-E7E3E3655317}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>HOURS:MINS</t>
+  </si>
+  <si>
+    <t>2020-10-13</t>
+  </si>
+  <si>
+    <t>16:35:52</t>
+  </si>
+  <si>
+    <t>16:35:54</t>
+  </si>
+  <si>
+    <t>0:0</t>
+  </si>
+  <si>
+    <t>16:36:00</t>
+  </si>
+  <si>
+    <t>16:36:02</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -48,95 +84,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -424,60 +408,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="n">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>44105</v>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>11:02:15</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>11:02:16</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>0:0</t>
-        </is>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more design tweeking, toggle entry field when forgot to clock in
</commit_message>
<xml_diff>
--- a/TimeInTimeOut.xlsx
+++ b/TimeInTimeOut.xlsx
@@ -1,81 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith Rich\Documents\PythonScripts\TimeCard\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EE7110-0FFD-443F-A20E-E7E3E3655317}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>OUT</t>
-  </si>
-  <si>
-    <t>HOURS:MINS</t>
-  </si>
-  <si>
-    <t>2020-10-13</t>
-  </si>
-  <si>
-    <t>16:35:52</t>
-  </si>
-  <si>
-    <t>16:35:54</t>
-  </si>
-  <si>
-    <t>0:0</t>
-  </si>
-  <si>
-    <t>16:36:00</t>
-  </si>
-  <si>
-    <t>16:36:02</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -98,29 +64,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -408,68 +443,763 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col width="10.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="8.140625" bestFit="1" customWidth="1" min="2" max="3"/>
+    <col width="12.7109375" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
+    <row r="2">
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2020-10-13</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>16:35:52</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>16:35:54</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>2020-10-13</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>16:36:00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>16:36:02</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-20</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>13:18:25</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>13:18:26</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-20</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>13:19:08</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>13:19:08</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-20</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>13:27:49</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>13:27:50</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-20</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>13:33:05</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>13:33:06</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-20</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>13:36:40</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>13:36:40</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-20</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16:06:26</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>16:06:27</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-20</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>16:07:35</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>16:07:36</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>16:16:12</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>16:16:13</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-20</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>16:17:30</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>16:17:32</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-20</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>16:17:30</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>16:17:35</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-21</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>08:29:46</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>08:29:46</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-21</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>08:29:46</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>08:29:47</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-21</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>08:29:51</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>08:29:51</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-21</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>08:33:16</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>08:33:17</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-21</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>09:49:10</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>09:49:10</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-21</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>10:01:44</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>10:01:44</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-22</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>11:57:04</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>11:57:06</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up some .bind commands and some other logic
</commit_message>
<xml_diff>
--- a/TimeInTimeOut.xlsx
+++ b/TimeInTimeOut.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D39"/>
+  <dimension ref="A2:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
@@ -1202,6 +1202,84 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="B40" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-22</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>15:26:31</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>15:26:32</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-22</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>15:26:31</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>15:26:33</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Preload text disapears when clicked correctly now. more logiv adjustments with weather or not a time is valid or not
</commit_message>
<xml_diff>
--- a/TimeInTimeOut.xlsx
+++ b/TimeInTimeOut.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D43"/>
+  <dimension ref="A2:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
@@ -1280,6 +1280,84 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="B44" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-23</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>11:36:41</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>11:36:41</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>HOURS:MINS</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>2020-10-23</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>11:55:49</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>31:3187</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>